<commit_message>
added amazon test project
</commit_message>
<xml_diff>
--- a/SELENIUM_RESOURCES/TestData/sampleData.xlsx
+++ b/SELENIUM_RESOURCES/TestData/sampleData.xlsx
@@ -19,19 +19,19 @@
     <t>ScenarioName</t>
   </si>
   <si>
-    <t>SearchText</t>
-  </si>
-  <si>
-    <t>scenario1</t>
-  </si>
-  <si>
-    <t>appium</t>
-  </si>
-  <si>
-    <t>selenium</t>
-  </si>
-  <si>
-    <t>scenario2</t>
+    <t>KindleEBook</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
   </si>
 </sst>
 </file>
@@ -373,40 +373,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>